<commit_message>
try adding affiex blueprint
</commit_message>
<xml_diff>
--- a/MoYu/Apis/MoYu.Api/Data/DataInput.xlsx
+++ b/MoYu/Apis/MoYu.Api/Data/DataInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\moyu\MoYu\Apis\MoYu.Api\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999DF655-44CC-4580-8E44-AB8A35C6CD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B9BAE3-002D-4E7B-BA60-FCBE2C7A9992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,7 +578,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -769,7 +771,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,11 +1528,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48217058-2D48-4338-92F5-A0F8187528A5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" xr:uid="{812A1E82-5967-4A5B-838C-A9E4B3613F15}">
+          <x14:formula1>
+            <xm:f>ItemType!$A$1:$A$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1636,7 +1652,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A14"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>